<commit_message>
Update CHESS RUSH PROJECT - DB.xlsx
</commit_message>
<xml_diff>
--- a/docs/CHESS RUSH PROJECT - DB.xlsx
+++ b/docs/CHESS RUSH PROJECT - DB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romtoni\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Server\Application\xampp_uptodate\htdocs\ChessRushSimulator\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2323,7 +2323,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G9" sqref="G9"/>
+      <selection pane="topRight" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2332,9 +2332,9 @@
     <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2351,20 +2351,20 @@
       <c r="D1" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="E1" s="80" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="57" t="s">
+        <v>253</v>
+      </c>
+      <c r="F1" s="80" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="50" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="54" t="s">
+      <c r="H1" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="54" t="s">
         <v>250</v>
-      </c>
-      <c r="I1" s="57" t="s">
-        <v>253</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>31</v>
@@ -2390,19 +2390,19 @@
         <v>1</v>
       </c>
       <c r="E2" s="52">
+        <v>1</v>
+      </c>
+      <c r="F2" s="52">
         <v>5</v>
       </c>
-      <c r="F2" s="9">
-        <v>0</v>
-      </c>
-      <c r="G2" s="52">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0</v>
-      </c>
-      <c r="I2" s="52">
-        <v>1</v>
+      <c r="G2" s="9">
+        <v>0</v>
+      </c>
+      <c r="H2" s="52">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0</v>
       </c>
       <c r="J2" s="9">
         <v>6</v>
@@ -2428,19 +2428,19 @@
         <v>2</v>
       </c>
       <c r="E3" s="11">
+        <v>4</v>
+      </c>
+      <c r="F3" s="11">
         <v>6</v>
       </c>
-      <c r="F3" s="9">
-        <v>0</v>
-      </c>
-      <c r="G3" s="11">
-        <v>1</v>
-      </c>
-      <c r="H3" s="9">
-        <v>0</v>
-      </c>
-      <c r="I3" s="11">
-        <v>4</v>
+      <c r="G3" s="9">
+        <v>0</v>
+      </c>
+      <c r="H3" s="11">
+        <v>1</v>
+      </c>
+      <c r="I3" s="9">
+        <v>0</v>
       </c>
       <c r="J3" s="9">
         <v>1</v>
@@ -2466,19 +2466,19 @@
         <v>3</v>
       </c>
       <c r="E4" s="11">
+        <v>1</v>
+      </c>
+      <c r="F4" s="11">
         <v>4</v>
       </c>
-      <c r="F4" s="9">
-        <v>0</v>
-      </c>
-      <c r="G4" s="11">
-        <v>2</v>
-      </c>
-      <c r="H4" s="9">
-        <v>0</v>
-      </c>
-      <c r="I4" s="11">
-        <v>1</v>
+      <c r="G4" s="9">
+        <v>0</v>
+      </c>
+      <c r="H4" s="11">
+        <v>2</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0</v>
       </c>
       <c r="J4" s="9">
         <v>1</v>
@@ -2504,19 +2504,19 @@
         <v>4</v>
       </c>
       <c r="E5" s="11">
+        <v>3</v>
+      </c>
+      <c r="F5" s="11">
         <v>7</v>
       </c>
-      <c r="F5" s="9">
-        <v>0</v>
-      </c>
-      <c r="G5" s="11">
+      <c r="G5" s="9">
+        <v>0</v>
+      </c>
+      <c r="H5" s="11">
         <v>4</v>
       </c>
-      <c r="H5" s="9">
-        <v>0</v>
-      </c>
-      <c r="I5" s="11">
-        <v>3</v>
+      <c r="I5" s="9">
+        <v>0</v>
       </c>
       <c r="J5" s="9">
         <v>6</v>
@@ -2541,20 +2541,20 @@
       <c r="D6" s="9">
         <v>5</v>
       </c>
-      <c r="E6" s="11">
-        <v>1</v>
-      </c>
-      <c r="F6" s="9">
+      <c r="E6" s="28">
+        <v>4</v>
+      </c>
+      <c r="F6" s="11">
+        <v>1</v>
+      </c>
+      <c r="G6" s="9">
         <v>11</v>
       </c>
-      <c r="G6" s="11">
+      <c r="H6" s="11">
         <v>4</v>
       </c>
-      <c r="H6" s="9">
-        <v>0</v>
-      </c>
-      <c r="I6" s="28">
-        <v>4</v>
+      <c r="I6" s="9">
+        <v>0</v>
       </c>
       <c r="J6" s="9">
         <v>1</v>
@@ -2582,17 +2582,17 @@
       <c r="E7" s="11">
         <v>2</v>
       </c>
-      <c r="F7" s="9">
-        <v>0</v>
-      </c>
-      <c r="G7" s="11">
+      <c r="F7" s="11">
+        <v>2</v>
+      </c>
+      <c r="G7" s="9">
+        <v>0</v>
+      </c>
+      <c r="H7" s="11">
         <v>8</v>
       </c>
-      <c r="H7" s="9">
-        <v>0</v>
-      </c>
-      <c r="I7" s="11">
-        <v>2</v>
+      <c r="I7" s="9">
+        <v>0</v>
       </c>
       <c r="J7" s="9">
         <v>6</v>
@@ -2620,17 +2620,17 @@
       <c r="E8" s="11">
         <v>2</v>
       </c>
-      <c r="F8" s="9">
-        <v>0</v>
-      </c>
-      <c r="G8" s="11">
+      <c r="F8" s="11">
+        <v>2</v>
+      </c>
+      <c r="G8" s="9">
+        <v>0</v>
+      </c>
+      <c r="H8" s="11">
         <v>8</v>
       </c>
-      <c r="H8" s="9">
-        <v>0</v>
-      </c>
-      <c r="I8" s="11">
-        <v>2</v>
+      <c r="I8" s="9">
+        <v>0</v>
       </c>
       <c r="J8" s="9">
         <v>6</v>
@@ -2656,19 +2656,19 @@
         <v>8</v>
       </c>
       <c r="E9" s="11">
+        <v>1</v>
+      </c>
+      <c r="F9" s="11">
         <v>7</v>
       </c>
-      <c r="F9" s="9">
-        <v>0</v>
-      </c>
-      <c r="G9" s="11">
+      <c r="G9" s="9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="11">
         <v>5</v>
       </c>
-      <c r="H9" s="9">
-        <v>0</v>
-      </c>
-      <c r="I9" s="11">
-        <v>1</v>
+      <c r="I9" s="9">
+        <v>0</v>
       </c>
       <c r="J9" s="9">
         <v>1</v>
@@ -2694,19 +2694,19 @@
         <v>9</v>
       </c>
       <c r="E10" s="11">
+        <v>2</v>
+      </c>
+      <c r="F10" s="11">
         <v>5</v>
       </c>
-      <c r="F10" s="9">
-        <v>0</v>
-      </c>
-      <c r="G10" s="11">
+      <c r="G10" s="9">
+        <v>0</v>
+      </c>
+      <c r="H10" s="11">
         <v>5</v>
       </c>
-      <c r="H10" s="9">
-        <v>0</v>
-      </c>
-      <c r="I10" s="11">
-        <v>2</v>
+      <c r="I10" s="9">
+        <v>0</v>
       </c>
       <c r="J10" s="9">
         <v>1</v>
@@ -2732,19 +2732,19 @@
         <v>10</v>
       </c>
       <c r="E11" s="11">
-        <v>1</v>
-      </c>
-      <c r="F11" s="9">
-        <v>0</v>
-      </c>
-      <c r="G11" s="11">
-        <v>3</v>
-      </c>
-      <c r="H11" s="9">
-        <v>0</v>
-      </c>
-      <c r="I11" s="11">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="F11" s="11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="9">
+        <v>0</v>
+      </c>
+      <c r="H11" s="11">
+        <v>3</v>
+      </c>
+      <c r="I11" s="9">
+        <v>0</v>
       </c>
       <c r="J11" s="9">
         <v>1</v>
@@ -2770,19 +2770,19 @@
         <v>11</v>
       </c>
       <c r="E12" s="11">
-        <v>2</v>
-      </c>
-      <c r="F12" s="9">
-        <v>0</v>
-      </c>
-      <c r="G12" s="11">
+        <v>3</v>
+      </c>
+      <c r="F12" s="11">
+        <v>2</v>
+      </c>
+      <c r="G12" s="9">
+        <v>0</v>
+      </c>
+      <c r="H12" s="11">
         <v>5</v>
       </c>
-      <c r="H12" s="9">
-        <v>0</v>
-      </c>
-      <c r="I12" s="11">
-        <v>3</v>
+      <c r="I12" s="9">
+        <v>0</v>
       </c>
       <c r="J12" s="9">
         <v>1</v>
@@ -2810,17 +2810,17 @@
       <c r="E13" s="11">
         <v>1</v>
       </c>
-      <c r="F13" s="9">
-        <v>0</v>
-      </c>
-      <c r="G13" s="11">
-        <v>3</v>
-      </c>
-      <c r="H13" s="9">
-        <v>0</v>
-      </c>
-      <c r="I13" s="11">
-        <v>1</v>
+      <c r="F13" s="11">
+        <v>1</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0</v>
+      </c>
+      <c r="H13" s="11">
+        <v>3</v>
+      </c>
+      <c r="I13" s="9">
+        <v>0</v>
       </c>
       <c r="J13" s="9">
         <v>1</v>
@@ -2846,19 +2846,19 @@
         <v>13</v>
       </c>
       <c r="E14" s="11">
+        <v>2</v>
+      </c>
+      <c r="F14" s="11">
         <v>8</v>
       </c>
-      <c r="F14" s="9">
-        <v>0</v>
-      </c>
-      <c r="G14" s="11">
-        <v>1</v>
-      </c>
-      <c r="H14" s="9">
-        <v>0</v>
-      </c>
-      <c r="I14" s="11">
-        <v>2</v>
+      <c r="G14" s="9">
+        <v>0</v>
+      </c>
+      <c r="H14" s="11">
+        <v>1</v>
+      </c>
+      <c r="I14" s="9">
+        <v>0</v>
       </c>
       <c r="J14" s="9">
         <v>6</v>
@@ -2884,19 +2884,19 @@
         <v>14</v>
       </c>
       <c r="E15" s="11">
-        <v>1</v>
-      </c>
-      <c r="F15" s="9">
-        <v>0</v>
-      </c>
-      <c r="G15" s="11">
-        <v>1</v>
-      </c>
-      <c r="H15" s="9">
-        <v>0</v>
-      </c>
-      <c r="I15" s="11">
         <v>4</v>
+      </c>
+      <c r="F15" s="11">
+        <v>1</v>
+      </c>
+      <c r="G15" s="9">
+        <v>0</v>
+      </c>
+      <c r="H15" s="11">
+        <v>1</v>
+      </c>
+      <c r="I15" s="9">
+        <v>0</v>
       </c>
       <c r="J15" s="9">
         <v>6</v>
@@ -2922,19 +2922,19 @@
         <v>15</v>
       </c>
       <c r="E16" s="11">
+        <v>2</v>
+      </c>
+      <c r="F16" s="11">
         <v>7</v>
       </c>
-      <c r="F16" s="9">
-        <v>0</v>
-      </c>
-      <c r="G16" s="11">
-        <v>1</v>
-      </c>
-      <c r="H16" s="9">
-        <v>0</v>
-      </c>
-      <c r="I16" s="11">
-        <v>2</v>
+      <c r="G16" s="9">
+        <v>0</v>
+      </c>
+      <c r="H16" s="11">
+        <v>1</v>
+      </c>
+      <c r="I16" s="9">
+        <v>0</v>
       </c>
       <c r="J16" s="9">
         <v>6</v>
@@ -2960,19 +2960,19 @@
         <v>16</v>
       </c>
       <c r="E17" s="11">
+        <v>2</v>
+      </c>
+      <c r="F17" s="11">
         <v>4</v>
       </c>
-      <c r="F17" s="9">
-        <v>0</v>
-      </c>
-      <c r="G17" s="11">
+      <c r="G17" s="9">
+        <v>0</v>
+      </c>
+      <c r="H17" s="11">
         <v>7</v>
       </c>
-      <c r="H17" s="9">
-        <v>0</v>
-      </c>
-      <c r="I17" s="11">
-        <v>2</v>
+      <c r="I17" s="9">
+        <v>0</v>
       </c>
       <c r="J17" s="9">
         <v>6</v>
@@ -2998,19 +2998,19 @@
         <v>17</v>
       </c>
       <c r="E18" s="11">
+        <v>4</v>
+      </c>
+      <c r="F18" s="11">
         <v>12</v>
       </c>
-      <c r="F18" s="9">
-        <v>0</v>
-      </c>
-      <c r="G18" s="11">
+      <c r="G18" s="9">
+        <v>0</v>
+      </c>
+      <c r="H18" s="11">
         <v>8</v>
       </c>
-      <c r="H18" s="9">
-        <v>0</v>
-      </c>
-      <c r="I18" s="11">
-        <v>4</v>
+      <c r="I18" s="9">
+        <v>0</v>
       </c>
       <c r="J18" s="9">
         <v>0</v>
@@ -3036,19 +3036,19 @@
         <v>18</v>
       </c>
       <c r="E19" s="11">
+        <v>3</v>
+      </c>
+      <c r="F19" s="11">
         <v>6</v>
       </c>
-      <c r="F19" s="9">
-        <v>0</v>
-      </c>
-      <c r="G19" s="11">
-        <v>2</v>
-      </c>
-      <c r="H19" s="9">
-        <v>0</v>
-      </c>
-      <c r="I19" s="11">
-        <v>3</v>
+      <c r="G19" s="9">
+        <v>0</v>
+      </c>
+      <c r="H19" s="11">
+        <v>2</v>
+      </c>
+      <c r="I19" s="9">
+        <v>0</v>
       </c>
       <c r="J19" s="9">
         <v>1</v>
@@ -3074,19 +3074,19 @@
         <v>19</v>
       </c>
       <c r="E20" s="11">
-        <v>2</v>
-      </c>
-      <c r="F20" s="9">
-        <v>0</v>
-      </c>
-      <c r="G20" s="11">
+        <v>1</v>
+      </c>
+      <c r="F20" s="11">
+        <v>2</v>
+      </c>
+      <c r="G20" s="9">
+        <v>0</v>
+      </c>
+      <c r="H20" s="11">
         <v>4</v>
       </c>
-      <c r="H20" s="9">
+      <c r="I20" s="9">
         <v>5</v>
-      </c>
-      <c r="I20" s="11">
-        <v>1</v>
       </c>
       <c r="J20" s="9">
         <v>6</v>
@@ -3114,17 +3114,17 @@
       <c r="E21" s="11">
         <v>3</v>
       </c>
-      <c r="F21" s="9">
-        <v>0</v>
-      </c>
-      <c r="G21" s="11">
-        <v>2</v>
-      </c>
-      <c r="H21" s="9">
-        <v>0</v>
-      </c>
-      <c r="I21" s="11">
-        <v>3</v>
+      <c r="F21" s="11">
+        <v>3</v>
+      </c>
+      <c r="G21" s="9">
+        <v>0</v>
+      </c>
+      <c r="H21" s="11">
+        <v>2</v>
+      </c>
+      <c r="I21" s="9">
+        <v>0</v>
       </c>
       <c r="J21" s="9">
         <v>1</v>
@@ -3150,19 +3150,19 @@
         <v>21</v>
       </c>
       <c r="E22" s="11">
-        <v>3</v>
-      </c>
-      <c r="F22" s="9">
-        <v>0</v>
-      </c>
-      <c r="G22" s="11">
-        <v>1</v>
-      </c>
-      <c r="H22" s="9">
-        <v>0</v>
-      </c>
-      <c r="I22" s="11">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="F22" s="11">
+        <v>3</v>
+      </c>
+      <c r="G22" s="9">
+        <v>0</v>
+      </c>
+      <c r="H22" s="11">
+        <v>1</v>
+      </c>
+      <c r="I22" s="9">
+        <v>0</v>
       </c>
       <c r="J22" s="9">
         <v>6</v>
@@ -3188,19 +3188,19 @@
         <v>22</v>
       </c>
       <c r="E23" s="11">
+        <v>5</v>
+      </c>
+      <c r="F23" s="11">
         <v>9</v>
       </c>
-      <c r="F23" s="9">
-        <v>0</v>
-      </c>
-      <c r="G23" s="11">
+      <c r="G23" s="9">
+        <v>0</v>
+      </c>
+      <c r="H23" s="11">
         <v>5</v>
       </c>
-      <c r="H23" s="9">
-        <v>0</v>
-      </c>
-      <c r="I23" s="11">
-        <v>5</v>
+      <c r="I23" s="9">
+        <v>0</v>
       </c>
       <c r="J23" s="9">
         <v>6</v>
@@ -3226,19 +3226,19 @@
         <v>23</v>
       </c>
       <c r="E24" s="11">
+        <v>4</v>
+      </c>
+      <c r="F24" s="11">
         <v>9</v>
       </c>
-      <c r="F24" s="9">
-        <v>0</v>
-      </c>
-      <c r="G24" s="11">
+      <c r="G24" s="9">
+        <v>0</v>
+      </c>
+      <c r="H24" s="11">
         <v>5</v>
       </c>
-      <c r="H24" s="9">
-        <v>0</v>
-      </c>
-      <c r="I24" s="11">
-        <v>4</v>
+      <c r="I24" s="9">
+        <v>0</v>
       </c>
       <c r="J24" s="9">
         <v>1</v>
@@ -3264,19 +3264,19 @@
         <v>24</v>
       </c>
       <c r="E25" s="11">
-        <v>1</v>
-      </c>
-      <c r="F25" s="9">
-        <v>0</v>
-      </c>
-      <c r="G25" s="11">
-        <v>3</v>
-      </c>
-      <c r="H25" s="9">
-        <v>0</v>
-      </c>
-      <c r="I25" s="11">
         <v>4</v>
+      </c>
+      <c r="F25" s="11">
+        <v>1</v>
+      </c>
+      <c r="G25" s="9">
+        <v>0</v>
+      </c>
+      <c r="H25" s="11">
+        <v>3</v>
+      </c>
+      <c r="I25" s="9">
+        <v>0</v>
       </c>
       <c r="J25" s="9">
         <v>1</v>
@@ -3302,19 +3302,19 @@
         <v>25</v>
       </c>
       <c r="E26" s="11">
+        <v>2</v>
+      </c>
+      <c r="F26" s="11">
         <v>8</v>
       </c>
-      <c r="F26" s="9">
-        <v>0</v>
-      </c>
-      <c r="G26" s="11">
-        <v>2</v>
-      </c>
-      <c r="H26" s="9">
-        <v>0</v>
-      </c>
-      <c r="I26" s="11">
-        <v>2</v>
+      <c r="G26" s="9">
+        <v>0</v>
+      </c>
+      <c r="H26" s="11">
+        <v>2</v>
+      </c>
+      <c r="I26" s="9">
+        <v>0</v>
       </c>
       <c r="J26" s="9">
         <v>1</v>
@@ -3340,19 +3340,19 @@
         <v>26</v>
       </c>
       <c r="E27" s="11">
-        <v>3</v>
-      </c>
-      <c r="F27" s="9">
-        <v>0</v>
-      </c>
-      <c r="G27" s="11">
+        <v>2</v>
+      </c>
+      <c r="F27" s="11">
+        <v>3</v>
+      </c>
+      <c r="G27" s="9">
+        <v>0</v>
+      </c>
+      <c r="H27" s="11">
         <v>6</v>
       </c>
-      <c r="H27" s="9">
-        <v>0</v>
-      </c>
-      <c r="I27" s="11">
-        <v>2</v>
+      <c r="I27" s="9">
+        <v>0</v>
       </c>
       <c r="J27" s="9">
         <v>1</v>
@@ -3378,19 +3378,19 @@
         <v>27</v>
       </c>
       <c r="E28" s="11">
+        <v>4</v>
+      </c>
+      <c r="F28" s="11">
         <v>7</v>
       </c>
-      <c r="F28" s="9">
-        <v>0</v>
-      </c>
-      <c r="G28" s="11">
+      <c r="G28" s="9">
+        <v>0</v>
+      </c>
+      <c r="H28" s="11">
         <v>6</v>
       </c>
-      <c r="H28" s="9">
-        <v>0</v>
-      </c>
-      <c r="I28" s="11">
-        <v>4</v>
+      <c r="I28" s="9">
+        <v>0</v>
       </c>
       <c r="J28" s="9">
         <v>6</v>
@@ -3416,19 +3416,19 @@
         <v>28</v>
       </c>
       <c r="E29" s="11">
+        <v>1</v>
+      </c>
+      <c r="F29" s="11">
         <v>4</v>
       </c>
-      <c r="F29" s="9">
-        <v>0</v>
-      </c>
-      <c r="G29" s="11">
+      <c r="G29" s="9">
+        <v>0</v>
+      </c>
+      <c r="H29" s="11">
         <v>7</v>
       </c>
-      <c r="H29" s="9">
-        <v>0</v>
-      </c>
-      <c r="I29" s="11">
-        <v>1</v>
+      <c r="I29" s="9">
+        <v>0</v>
       </c>
       <c r="J29" s="9">
         <v>6</v>
@@ -3456,17 +3456,17 @@
       <c r="E30" s="11">
         <v>2</v>
       </c>
-      <c r="F30" s="9">
+      <c r="F30" s="11">
+        <v>2</v>
+      </c>
+      <c r="G30" s="9">
         <v>11</v>
       </c>
-      <c r="G30" s="11">
-        <v>3</v>
-      </c>
-      <c r="H30" s="9">
-        <v>0</v>
-      </c>
-      <c r="I30" s="11">
-        <v>2</v>
+      <c r="H30" s="11">
+        <v>3</v>
+      </c>
+      <c r="I30" s="9">
+        <v>0</v>
       </c>
       <c r="J30" s="9">
         <v>1</v>
@@ -3492,19 +3492,19 @@
         <v>30</v>
       </c>
       <c r="E31" s="11">
+        <v>3</v>
+      </c>
+      <c r="F31" s="11">
         <v>8</v>
       </c>
-      <c r="F31" s="9">
-        <v>0</v>
-      </c>
-      <c r="G31" s="11">
+      <c r="G31" s="9">
+        <v>0</v>
+      </c>
+      <c r="H31" s="11">
         <v>6</v>
       </c>
-      <c r="H31" s="9">
-        <v>0</v>
-      </c>
-      <c r="I31" s="11">
-        <v>3</v>
+      <c r="I31" s="9">
+        <v>0</v>
       </c>
       <c r="J31" s="9">
         <v>1</v>
@@ -3530,19 +3530,19 @@
         <v>31</v>
       </c>
       <c r="E32" s="11">
-        <v>2</v>
-      </c>
-      <c r="F32" s="9">
-        <v>0</v>
-      </c>
-      <c r="G32" s="11">
+        <v>1</v>
+      </c>
+      <c r="F32" s="11">
+        <v>2</v>
+      </c>
+      <c r="G32" s="9">
+        <v>0</v>
+      </c>
+      <c r="H32" s="11">
         <v>9</v>
       </c>
-      <c r="H32" s="9">
-        <v>0</v>
-      </c>
-      <c r="I32" s="11">
-        <v>1</v>
+      <c r="I32" s="9">
+        <v>0</v>
       </c>
       <c r="J32" s="9">
         <v>1</v>
@@ -3568,19 +3568,19 @@
         <v>32</v>
       </c>
       <c r="E33" s="11">
-        <v>3</v>
-      </c>
-      <c r="F33" s="9">
-        <v>0</v>
-      </c>
-      <c r="G33" s="11">
+        <v>4</v>
+      </c>
+      <c r="F33" s="11">
+        <v>3</v>
+      </c>
+      <c r="G33" s="9">
+        <v>0</v>
+      </c>
+      <c r="H33" s="11">
         <v>8</v>
       </c>
-      <c r="H33" s="9">
-        <v>0</v>
-      </c>
-      <c r="I33" s="11">
-        <v>4</v>
+      <c r="I33" s="9">
+        <v>0</v>
       </c>
       <c r="J33" s="9">
         <v>1</v>
@@ -3606,19 +3606,19 @@
         <v>33</v>
       </c>
       <c r="E34" s="11">
+        <v>2</v>
+      </c>
+      <c r="F34" s="11">
         <v>8</v>
       </c>
-      <c r="F34" s="9">
-        <v>0</v>
-      </c>
-      <c r="G34" s="11">
+      <c r="G34" s="9">
+        <v>0</v>
+      </c>
+      <c r="H34" s="11">
         <v>4</v>
       </c>
-      <c r="H34" s="9">
-        <v>0</v>
-      </c>
-      <c r="I34" s="11">
-        <v>2</v>
+      <c r="I34" s="9">
+        <v>0</v>
       </c>
       <c r="J34" s="9">
         <v>6</v>
@@ -3644,19 +3644,19 @@
         <v>34</v>
       </c>
       <c r="E35" s="11">
+        <v>3</v>
+      </c>
+      <c r="F35" s="11">
         <v>9</v>
       </c>
-      <c r="F35" s="9">
-        <v>0</v>
-      </c>
-      <c r="G35" s="11">
-        <v>2</v>
-      </c>
-      <c r="H35" s="9">
-        <v>0</v>
-      </c>
-      <c r="I35" s="11">
-        <v>3</v>
+      <c r="G35" s="9">
+        <v>0</v>
+      </c>
+      <c r="H35" s="11">
+        <v>2</v>
+      </c>
+      <c r="I35" s="9">
+        <v>0</v>
       </c>
       <c r="J35" s="9">
         <v>1</v>
@@ -3682,19 +3682,19 @@
         <v>35</v>
       </c>
       <c r="E36" s="11">
+        <v>3</v>
+      </c>
+      <c r="F36" s="11">
         <v>4</v>
       </c>
-      <c r="F36" s="9">
-        <v>0</v>
-      </c>
-      <c r="G36" s="11">
+      <c r="G36" s="9">
+        <v>0</v>
+      </c>
+      <c r="H36" s="11">
         <v>5</v>
       </c>
-      <c r="H36" s="9">
-        <v>0</v>
-      </c>
-      <c r="I36" s="11">
-        <v>3</v>
+      <c r="I36" s="9">
+        <v>0</v>
       </c>
       <c r="J36" s="9">
         <v>1</v>
@@ -3720,19 +3720,19 @@
         <v>36</v>
       </c>
       <c r="E37" s="11">
+        <v>4</v>
+      </c>
+      <c r="F37" s="11">
         <v>5</v>
       </c>
-      <c r="F37" s="9">
-        <v>0</v>
-      </c>
-      <c r="G37" s="11">
-        <v>3</v>
-      </c>
-      <c r="H37" s="9">
-        <v>0</v>
-      </c>
-      <c r="I37" s="11">
-        <v>4</v>
+      <c r="G37" s="9">
+        <v>0</v>
+      </c>
+      <c r="H37" s="11">
+        <v>3</v>
+      </c>
+      <c r="I37" s="9">
+        <v>0</v>
       </c>
       <c r="J37" s="9">
         <v>6</v>
@@ -3758,19 +3758,19 @@
         <v>37</v>
       </c>
       <c r="E38" s="11">
+        <v>1</v>
+      </c>
+      <c r="F38" s="11">
         <v>4</v>
       </c>
-      <c r="F38" s="9">
-        <v>0</v>
-      </c>
-      <c r="G38" s="11">
+      <c r="G38" s="9">
+        <v>0</v>
+      </c>
+      <c r="H38" s="11">
         <v>7</v>
       </c>
-      <c r="H38" s="9">
-        <v>0</v>
-      </c>
-      <c r="I38" s="11">
-        <v>1</v>
+      <c r="I38" s="9">
+        <v>0</v>
       </c>
       <c r="J38" s="9">
         <v>6</v>
@@ -3796,19 +3796,19 @@
         <v>38</v>
       </c>
       <c r="E39" s="11">
-        <v>2</v>
-      </c>
-      <c r="F39" s="9">
+        <v>3</v>
+      </c>
+      <c r="F39" s="11">
+        <v>2</v>
+      </c>
+      <c r="G39" s="9">
         <v>7</v>
       </c>
-      <c r="G39" s="11">
-        <v>2</v>
-      </c>
-      <c r="H39" s="9">
-        <v>0</v>
-      </c>
-      <c r="I39" s="11">
-        <v>3</v>
+      <c r="H39" s="11">
+        <v>2</v>
+      </c>
+      <c r="I39" s="9">
+        <v>0</v>
       </c>
       <c r="J39" s="9">
         <v>1</v>
@@ -3834,19 +3834,19 @@
         <v>39</v>
       </c>
       <c r="E40" s="11">
-        <v>2</v>
-      </c>
-      <c r="F40" s="9">
-        <v>0</v>
-      </c>
-      <c r="G40" s="11">
-        <v>2</v>
-      </c>
-      <c r="H40" s="9">
-        <v>0</v>
-      </c>
-      <c r="I40" s="11">
         <v>4</v>
+      </c>
+      <c r="F40" s="11">
+        <v>2</v>
+      </c>
+      <c r="G40" s="9">
+        <v>0</v>
+      </c>
+      <c r="H40" s="11">
+        <v>2</v>
+      </c>
+      <c r="I40" s="9">
+        <v>0</v>
       </c>
       <c r="J40" s="9">
         <v>1</v>
@@ -3872,19 +3872,19 @@
         <v>40</v>
       </c>
       <c r="E41" s="11">
-        <v>1</v>
-      </c>
-      <c r="F41" s="9">
-        <v>0</v>
-      </c>
-      <c r="G41" s="11">
+        <v>3</v>
+      </c>
+      <c r="F41" s="11">
+        <v>1</v>
+      </c>
+      <c r="G41" s="9">
+        <v>0</v>
+      </c>
+      <c r="H41" s="11">
         <v>4</v>
       </c>
-      <c r="H41" s="9">
-        <v>0</v>
-      </c>
-      <c r="I41" s="11">
-        <v>3</v>
+      <c r="I41" s="9">
+        <v>0</v>
       </c>
       <c r="J41" s="9">
         <v>6</v>
@@ -3910,19 +3910,19 @@
         <v>41</v>
       </c>
       <c r="E42" s="11">
+        <v>5</v>
+      </c>
+      <c r="F42" s="11">
         <v>4</v>
       </c>
-      <c r="F42" s="9">
-        <v>0</v>
-      </c>
-      <c r="G42" s="11">
+      <c r="G42" s="9">
+        <v>0</v>
+      </c>
+      <c r="H42" s="11">
         <v>7</v>
       </c>
-      <c r="H42" s="9">
-        <v>0</v>
-      </c>
-      <c r="I42" s="11">
-        <v>5</v>
+      <c r="I42" s="9">
+        <v>0</v>
       </c>
       <c r="J42" s="9">
         <v>1</v>
@@ -3948,19 +3948,19 @@
         <v>42</v>
       </c>
       <c r="E43" s="11">
+        <v>5</v>
+      </c>
+      <c r="F43" s="11">
         <v>7</v>
       </c>
-      <c r="F43" s="9">
-        <v>0</v>
-      </c>
-      <c r="G43" s="11">
-        <v>3</v>
-      </c>
-      <c r="H43" s="9">
-        <v>0</v>
-      </c>
-      <c r="I43" s="11">
-        <v>5</v>
+      <c r="G43" s="9">
+        <v>0</v>
+      </c>
+      <c r="H43" s="11">
+        <v>3</v>
+      </c>
+      <c r="I43" s="9">
+        <v>0</v>
       </c>
       <c r="J43" s="9">
         <v>1</v>
@@ -3986,19 +3986,19 @@
         <v>43</v>
       </c>
       <c r="E44" s="11">
+        <v>3</v>
+      </c>
+      <c r="F44" s="11">
         <v>8</v>
       </c>
-      <c r="F44" s="9">
-        <v>0</v>
-      </c>
-      <c r="G44" s="11">
+      <c r="G44" s="9">
+        <v>0</v>
+      </c>
+      <c r="H44" s="11">
         <v>9</v>
       </c>
-      <c r="H44" s="9">
-        <v>0</v>
-      </c>
-      <c r="I44" s="11">
-        <v>3</v>
+      <c r="I44" s="9">
+        <v>0</v>
       </c>
       <c r="J44" s="9">
         <v>1</v>
@@ -4024,19 +4024,19 @@
         <v>44</v>
       </c>
       <c r="E45" s="11">
+        <v>4</v>
+      </c>
+      <c r="F45" s="11">
         <v>8</v>
       </c>
-      <c r="F45" s="9">
-        <v>0</v>
-      </c>
-      <c r="G45" s="11">
-        <v>1</v>
-      </c>
-      <c r="H45" s="9">
-        <v>0</v>
-      </c>
-      <c r="I45" s="11">
-        <v>4</v>
+      <c r="G45" s="9">
+        <v>0</v>
+      </c>
+      <c r="H45" s="11">
+        <v>1</v>
+      </c>
+      <c r="I45" s="9">
+        <v>0</v>
       </c>
       <c r="J45" s="9">
         <v>6</v>
@@ -4062,19 +4062,19 @@
         <v>45</v>
       </c>
       <c r="E46" s="11">
+        <v>5</v>
+      </c>
+      <c r="F46" s="11">
         <v>4</v>
       </c>
-      <c r="F46" s="9">
-        <v>0</v>
-      </c>
-      <c r="G46" s="11">
+      <c r="G46" s="9">
+        <v>0</v>
+      </c>
+      <c r="H46" s="11">
         <v>7</v>
       </c>
-      <c r="H46" s="9">
-        <v>0</v>
-      </c>
-      <c r="I46" s="11">
-        <v>5</v>
+      <c r="I46" s="9">
+        <v>0</v>
       </c>
       <c r="J46" s="9">
         <v>6</v>
@@ -4100,19 +4100,19 @@
         <v>46</v>
       </c>
       <c r="E47" s="11">
+        <v>1</v>
+      </c>
+      <c r="F47" s="11">
         <v>6</v>
       </c>
-      <c r="F47" s="9">
-        <v>0</v>
-      </c>
-      <c r="G47" s="11">
-        <v>3</v>
-      </c>
-      <c r="H47" s="9">
-        <v>0</v>
-      </c>
-      <c r="I47" s="11">
-        <v>1</v>
+      <c r="G47" s="9">
+        <v>0</v>
+      </c>
+      <c r="H47" s="11">
+        <v>3</v>
+      </c>
+      <c r="I47" s="9">
+        <v>0</v>
       </c>
       <c r="J47" s="9">
         <v>1</v>
@@ -4140,17 +4140,17 @@
       <c r="E48" s="11">
         <v>2</v>
       </c>
-      <c r="F48" s="9">
-        <v>0</v>
-      </c>
-      <c r="G48" s="11">
+      <c r="F48" s="11">
+        <v>2</v>
+      </c>
+      <c r="G48" s="9">
+        <v>0</v>
+      </c>
+      <c r="H48" s="11">
         <v>4</v>
       </c>
-      <c r="H48" s="9">
-        <v>0</v>
-      </c>
-      <c r="I48" s="11">
-        <v>2</v>
+      <c r="I48" s="9">
+        <v>0</v>
       </c>
       <c r="J48" s="9">
         <v>6</v>
@@ -4178,17 +4178,17 @@
       <c r="E49" s="11">
         <v>3</v>
       </c>
-      <c r="F49" s="9">
+      <c r="F49" s="11">
+        <v>3</v>
+      </c>
+      <c r="G49" s="9">
         <v>11</v>
       </c>
-      <c r="G49" s="11">
-        <v>2</v>
-      </c>
-      <c r="H49" s="9">
-        <v>0</v>
-      </c>
-      <c r="I49" s="11">
-        <v>3</v>
+      <c r="H49" s="11">
+        <v>2</v>
+      </c>
+      <c r="I49" s="9">
+        <v>0</v>
       </c>
       <c r="J49" s="9">
         <v>1</v>
@@ -4214,19 +4214,19 @@
         <v>49</v>
       </c>
       <c r="E50" s="11">
+        <v>3</v>
+      </c>
+      <c r="F50" s="11">
         <v>10</v>
       </c>
-      <c r="F50" s="9">
-        <v>0</v>
-      </c>
-      <c r="G50" s="11">
-        <v>3</v>
-      </c>
-      <c r="H50" s="9">
-        <v>0</v>
-      </c>
-      <c r="I50" s="11">
-        <v>3</v>
+      <c r="G50" s="9">
+        <v>0</v>
+      </c>
+      <c r="H50" s="11">
+        <v>3</v>
+      </c>
+      <c r="I50" s="9">
+        <v>0</v>
       </c>
       <c r="J50" s="9">
         <v>6</v>
@@ -4252,19 +4252,19 @@
         <v>50</v>
       </c>
       <c r="E51" s="11">
+        <v>5</v>
+      </c>
+      <c r="F51" s="11">
         <v>10</v>
       </c>
-      <c r="F51" s="9">
-        <v>0</v>
-      </c>
-      <c r="G51" s="11">
+      <c r="G51" s="9">
+        <v>0</v>
+      </c>
+      <c r="H51" s="11">
         <v>6</v>
       </c>
-      <c r="H51" s="9">
-        <v>0</v>
-      </c>
-      <c r="I51" s="11">
-        <v>5</v>
+      <c r="I51" s="9">
+        <v>0</v>
       </c>
       <c r="J51" s="9">
         <v>6</v>
@@ -4290,19 +4290,19 @@
         <v>51</v>
       </c>
       <c r="E52" s="11">
+        <v>2</v>
+      </c>
+      <c r="F52" s="11">
         <v>6</v>
       </c>
-      <c r="F52" s="9">
-        <v>0</v>
-      </c>
-      <c r="G52" s="11">
+      <c r="G52" s="9">
+        <v>0</v>
+      </c>
+      <c r="H52" s="11">
         <v>6</v>
       </c>
-      <c r="H52" s="9">
-        <v>0</v>
-      </c>
-      <c r="I52" s="11">
-        <v>2</v>
+      <c r="I52" s="9">
+        <v>0</v>
       </c>
       <c r="J52" s="9">
         <v>6</v>
@@ -4328,19 +4328,19 @@
         <v>52</v>
       </c>
       <c r="E53" s="11">
-        <v>1</v>
-      </c>
-      <c r="F53" s="9">
-        <v>3</v>
-      </c>
-      <c r="G53" s="11">
-        <v>1</v>
-      </c>
-      <c r="H53" s="9">
-        <v>0</v>
-      </c>
-      <c r="I53" s="11">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="F53" s="11">
+        <v>1</v>
+      </c>
+      <c r="G53" s="9">
+        <v>3</v>
+      </c>
+      <c r="H53" s="11">
+        <v>1</v>
+      </c>
+      <c r="I53" s="9">
+        <v>0</v>
       </c>
       <c r="J53" s="9">
         <v>6</v>
@@ -4366,19 +4366,19 @@
         <v>53</v>
       </c>
       <c r="E54" s="11">
-        <v>3</v>
-      </c>
-      <c r="F54" s="9">
-        <v>0</v>
-      </c>
-      <c r="G54" s="11">
+        <v>1</v>
+      </c>
+      <c r="F54" s="11">
+        <v>3</v>
+      </c>
+      <c r="G54" s="9">
+        <v>0</v>
+      </c>
+      <c r="H54" s="11">
         <v>8</v>
       </c>
-      <c r="H54" s="9">
-        <v>0</v>
-      </c>
-      <c r="I54" s="11">
-        <v>1</v>
+      <c r="I54" s="9">
+        <v>0</v>
       </c>
       <c r="J54" s="9">
         <v>6</v>
@@ -4404,19 +4404,19 @@
         <v>54</v>
       </c>
       <c r="E55" s="53">
+        <v>2</v>
+      </c>
+      <c r="F55" s="53">
         <v>5</v>
       </c>
-      <c r="F55" s="6">
-        <v>0</v>
-      </c>
-      <c r="G55" s="53">
-        <v>1</v>
-      </c>
-      <c r="H55" s="6">
-        <v>0</v>
-      </c>
-      <c r="I55" s="53">
-        <v>2</v>
+      <c r="G55" s="6">
+        <v>0</v>
+      </c>
+      <c r="H55" s="53">
+        <v>1</v>
+      </c>
+      <c r="I55" s="6">
+        <v>0</v>
       </c>
       <c r="J55" s="6">
         <v>6</v>

</xml_diff>

<commit_message>
Prograss Phase 1 u1
- Fixing Minor Bugs
- Added View Temporary Build By Race
- Added View Temporary Build by Class
- Add PL/SQL to Find Synergy by Temporary Build
</commit_message>
<xml_diff>
--- a/docs/CHESS RUSH PROJECT - DB.xlsx
+++ b/docs/CHESS RUSH PROJECT - DB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="655" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="655" firstSheet="13" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="HERO" sheetId="1" r:id="rId1"/>
@@ -9996,8 +9996,8 @@
   </sheetPr>
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D44" sqref="D1:D44"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10739,7 +10739,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="23">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" s="24" t="s">
         <v>351</v>
@@ -10768,7 +10768,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="23">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B27" s="24" t="s">
         <v>353</v>
@@ -10797,7 +10797,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="23">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B28" s="24" t="s">
         <v>355</v>
@@ -10826,7 +10826,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="23">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B29" s="24" t="s">
         <v>357</v>
@@ -10855,7 +10855,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="23">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B30" s="24" t="s">
         <v>359</v>
@@ -10884,7 +10884,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="23">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B31" s="24" t="s">
         <v>361</v>
@@ -10913,7 +10913,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="23">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B32" s="24" t="s">
         <v>363</v>
@@ -10942,7 +10942,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="23">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B33" s="24" t="s">
         <v>365</v>
@@ -10971,7 +10971,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="23">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B34" s="24" t="s">
         <v>367</v>
@@ -11000,7 +11000,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="23">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B35" s="24" t="s">
         <v>369</v>
@@ -11029,7 +11029,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="23">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B36" s="24" t="s">
         <v>371</v>
@@ -11058,7 +11058,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="23">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B37" s="24" t="s">
         <v>373</v>
@@ -11087,7 +11087,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="23">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B38" s="24" t="s">
         <v>375</v>
@@ -11116,7 +11116,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="23">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B39" s="24" t="s">
         <v>377</v>
@@ -11145,7 +11145,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="23">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B40" s="24" t="s">
         <v>379</v>
@@ -11174,7 +11174,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="23">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B41" s="24" t="s">
         <v>381</v>
@@ -11203,7 +11203,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="23">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="B42" s="24" t="s">
         <v>383</v>
@@ -11232,7 +11232,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="23">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="B43" s="24" t="s">
         <v>385</v>
@@ -11260,8 +11260,8 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="21">
-        <v>24</v>
+      <c r="A44" s="23">
+        <v>43</v>
       </c>
       <c r="B44" s="26" t="s">
         <v>387</v>
@@ -17255,7 +17255,7 @@
   </sheetPr>
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="C4" sqref="C4"/>
     </sheetView>

</xml_diff>